<commit_message>
Add user engagement metrics
</commit_message>
<xml_diff>
--- a/list of app metrics to track.xlsx
+++ b/list of app metrics to track.xlsx
@@ -165,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -177,13 +177,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +207,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -215,6 +226,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -228,7 +261,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -237,7 +270,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -246,43 +279,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,28 +309,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -322,50 +370,56 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -385,8 +439,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -405,10 +461,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -585,11 +641,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -598,27 +657,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -875,10 +934,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1169,7 +1228,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1447,16 +1506,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G71"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="27.9062" style="1" customWidth="1"/>
-    <col min="2" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.0938" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7188" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1464,734 +1524,734 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="44.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" ht="26.7" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" t="s" s="7">
+      <c r="D3" s="10"/>
+      <c r="E3" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" ht="92.05" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s" s="10">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" ht="38.7" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" t="s" s="11">
+      <c r="D4" s="14"/>
+      <c r="E4" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" ht="80.05" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" t="s" s="10">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" ht="26.7" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" t="s" s="11">
+      <c r="D5" s="14"/>
+      <c r="E5" t="s" s="13">
         <v>15</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" ht="44.05" customHeight="1">
-      <c r="A6" t="s" s="13">
+      <c r="A6" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="B6" t="s" s="12">
         <v>17</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" ht="104.05" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" t="s" s="10">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" ht="38.7" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" t="s" s="12">
         <v>19</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" t="s" s="11">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" t="s" s="13">
         <v>20</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="56.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" t="s" s="10">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" ht="26.7" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" t="s" s="12">
         <v>21</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" t="s" s="11">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" ht="104.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" t="s" s="10">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" ht="38.7" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" t="s" s="12">
         <v>23</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" t="s" s="11">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" t="s" s="10">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" t="s" s="12">
         <v>25</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" ht="68.05" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" t="s" s="10">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" ht="26.7" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" t="s" s="12">
         <v>26</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" t="s" s="11">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="13">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="B12" t="s" s="10">
+      <c r="B12" t="s" s="12">
         <v>29</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" ht="32.05" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" t="s" s="10">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" s="11"/>
+      <c r="B13" t="s" s="12">
         <v>30</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" t="s" s="10">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" s="11"/>
+      <c r="B14" t="s" s="12">
         <v>31</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" t="s" s="13">
         <v>32</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" t="s" s="11">
+      <c r="D14" s="14"/>
+      <c r="E14" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="13">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" t="s" s="15">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="10">
+      <c r="B15" t="s" s="12">
         <v>35</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" ht="140.05" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s" s="10">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" ht="74.7" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" t="s" s="12">
         <v>36</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" t="s" s="11">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" t="s" s="13">
         <v>37</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" t="s" s="10">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" ht="14.7" customHeight="1">
+      <c r="A17" s="11"/>
+      <c r="B17" t="s" s="12">
         <v>38</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" ht="32.05" customHeight="1">
-      <c r="A18" t="s" s="13">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" ht="14.7" customHeight="1">
+      <c r="A18" t="s" s="15">
         <v>39</v>
       </c>
-      <c r="B18" t="s" s="10">
+      <c r="B18" t="s" s="12">
         <v>40</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" ht="32.05" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" t="s" s="10">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" ht="14.7" customHeight="1">
+      <c r="A19" s="11"/>
+      <c r="B19" t="s" s="12">
         <v>41</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" t="s" s="10">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" ht="14.7" customHeight="1">
+      <c r="A20" s="11"/>
+      <c r="B20" t="s" s="12">
         <v>42</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" ht="32.05" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" t="s" s="10">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" ht="14.7" customHeight="1">
+      <c r="A21" s="11"/>
+      <c r="B21" t="s" s="12">
         <v>43</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" ht="32.05" customHeight="1">
-      <c r="A22" t="s" s="13">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" ht="14.7" customHeight="1">
+      <c r="A22" t="s" s="15">
         <v>44</v>
       </c>
-      <c r="B22" t="s" s="10">
+      <c r="B22" t="s" s="12">
         <v>45</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" ht="32.05" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" t="s" s="10">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" ht="14.7" customHeight="1">
+      <c r="A23" s="11"/>
+      <c r="B23" t="s" s="12">
         <v>46</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
     </row>
     <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" s="9"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="9"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" s="9"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="9"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="9"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="9"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" s="9"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" s="9"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="9"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
     </row>
     <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" s="9"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" s="9"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" s="9"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="9"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" s="9"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" s="9"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" s="9"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" s="9"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
     </row>
     <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" s="9"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" s="9"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" s="9"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" s="9"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" s="9"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
     </row>
     <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" s="9"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" s="9"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" s="9"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" s="9"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
     </row>
     <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" s="9"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
     </row>
     <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" s="9"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
     </row>
     <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" s="9"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
     </row>
     <row r="66" ht="20.05" customHeight="1">
-      <c r="A66" s="9"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
     </row>
     <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" s="9"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
     </row>
     <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" s="9"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
     </row>
     <row r="69" ht="20.05" customHeight="1">
-      <c r="A69" s="9"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
     </row>
     <row r="70" ht="20.05" customHeight="1">
-      <c r="A70" s="9"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
     </row>
     <row r="71" ht="20.05" customHeight="1">
-      <c r="A71" s="9"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>